<commit_message>
keeping track of mpcs
</commit_message>
<xml_diff>
--- a/mpc_multiplier_THP_hutchins/keeping track of mpcs.xlsx
+++ b/mpc_multiplier_THP_hutchins/keeping track of mpcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\fim\mpc_multiplier_THP_hutchins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lstojanovic\Downloads\fim\mpc_multiplier_THP_hutchins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB33541-1524-4A3C-BC58-F63F8042C4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916FDA2-D86D-40AE-AD81-816AF82DB42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{A27480DD-A5B8-4B82-93DD-4AC96F7B666D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27480DD-A5B8-4B82-93DD-4AC96F7B666D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Name of data in projections df</t>
   </si>
@@ -117,15 +117,102 @@
       .names = "{.col}_post_mpc"
     ),</t>
   </si>
+  <si>
+    <t>state_ui_arp</t>
+  </si>
+  <si>
+    <t>federal_other_vulnerable_arp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    across(
+      .cols = all_of(
+        c("rebate_checks_arp", "federal_other_direct_aid_arp") %&gt;% paste0("_minus_neutral")
+      ),
+      #same as above, applying a different MPC function to these 
+      .fns = ~ mpc_direct_aid_arp(.),
+      .names = "{.col}_post_mpc"
+    ),</t>
+  </si>
+  <si>
+    <t>rebate_checks_arp</t>
+  </si>
+  <si>
+    <t>federal_other_direct_aid_arp</t>
+  </si>
+  <si>
+    <t>mpc_direct_aid_arp(.)</t>
+  </si>
+  <si>
+    <t>246-254</t>
+  </si>
+  <si>
+    <t>246-255</t>
+  </si>
+  <si>
+    <t>254-261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    across(
+      .cols = all_of(
+        c("federal_student_loans") %&gt;% paste0("_minus_neutral")
+      ),
+      #same as above, applying a different MPC function to these 
+      .fns = ~ mpc_student_loans(.),
+      .names = "{.col}_post_mpc"
+    ),</t>
+  </si>
+  <si>
+    <t>262-269</t>
+  </si>
+  <si>
+    <t>mpc_student_loans(.)</t>
+  </si>
+  <si>
+    <t>federal_student_loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    across(
+      .cols = any_of(
+        c("supply_side_ira") %&gt;% paste0("_minus_neutral")
+      ),
+      #getting the post mpc levels for the ARP variables
+      .fns = ~ mpc_supply_side_ira(.x),
+      .names = "{.col}_post_mpc"
+    ),</t>
+  </si>
+  <si>
+    <t>270-277</t>
+  </si>
+  <si>
+    <t>mpc_supply_side_ira(.x)</t>
+  </si>
+  <si>
+    <t>supply_side_ira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    #same as above, applying a different MPC function to this
+    federal_aid_to_small_businesses_arp_minus_neutral_post_mpc = 
+      mpc_small_businesses_arp ((federal_aid_to_small_businesses_arp_minus_neutral))
+  )</t>
+  </si>
+  <si>
+    <t>278-281</t>
+  </si>
+  <si>
+    <t>mpc_small_businesses_arp()</t>
+  </si>
+  <si>
+    <t>federal_aid_to_small_businesses</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +224,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,7 +258,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -486,14 +579,14 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
     <col min="4" max="4" width="19.7265625" style="4" customWidth="1"/>
     <col min="5" max="16" width="5.7265625" customWidth="1"/>
   </cols>
@@ -778,91 +871,277 @@
       <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="E9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.04</v>
+      </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.04</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.04</v>
+      </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.04</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E15" s="2"/>
+      <c r="A15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -876,18 +1155,54 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E17" s="2"/>
@@ -1002,6 +1317,7 @@
       <c r="P24" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update keeping track of mpcs.xlsx
</commit_message>
<xml_diff>
--- a/mpc_multiplier_THP_hutchins/keeping track of mpcs.xlsx
+++ b/mpc_multiplier_THP_hutchins/keeping track of mpcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lstojanovic\Downloads\fim\mpc_multiplier_THP_hutchins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916FDA2-D86D-40AE-AD81-816AF82DB42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C4DB4-12DF-43E2-B4E6-1CC30666C419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27480DD-A5B8-4B82-93DD-4AC96F7B666D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Name of data in projections df</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>federal_aid_to_small_businesses</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641F86AC-7062-43C5-B0BC-8200C937F957}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,13 +594,13 @@
     <col min="5" max="16" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D1" s="3"/>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
@@ -606,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,8 +658,11 @@
       <c r="P3" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -697,8 +703,12 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q4" s="2">
+        <f>SUM(E4:P4)</f>
+        <v>0.97999999999999976</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -735,8 +745,12 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q5" s="2">
+        <f t="shared" ref="Q5:Q16" si="0">SUM(E5:P5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -773,8 +787,12 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q6" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -815,8 +833,12 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -857,8 +879,12 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -899,8 +925,12 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -941,8 +971,12 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
@@ -983,8 +1017,12 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1033,8 +1071,12 @@
       <c r="P12" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71000000000000019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1083,8 +1125,12 @@
       <c r="P13" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7300000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -1125,8 +1171,12 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -1153,8 +1203,12 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q15" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1202,6 +1256,10 @@
       </c>
       <c r="P16" s="2">
         <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000011</v>
       </c>
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.35">

</xml_diff>